<commit_message>
INT-1140: Case rocket database connection
</commit_message>
<xml_diff>
--- a/db/postgres/data/intake_codes.xlsx
+++ b/db/postgres/data/intake_codes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CWS-NS3/cws_legacy/swagger/lov/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsmith/workspace/jobs/db/postgres/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$321</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$B$60</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1714,7 +1714,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1890,6 +1890,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2157,19 +2160,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R321"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="E328" sqref="E328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
@@ -2235,7 +2239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1068</v>
       </c>
@@ -2270,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1069</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1070</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1071</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1072</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1073</v>
       </c>
@@ -2430,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1074</v>
       </c>
@@ -2465,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1075</v>
       </c>
@@ -2497,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1076</v>
       </c>
@@ -2529,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1077</v>
       </c>
@@ -2564,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1078</v>
       </c>
@@ -2596,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1079</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1080</v>
       </c>
@@ -2660,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1081</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1082</v>
       </c>
@@ -2724,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1083</v>
       </c>
@@ -2756,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1084</v>
       </c>
@@ -2788,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1085</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1086</v>
       </c>
@@ -2852,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1087</v>
       </c>
@@ -2884,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1088</v>
       </c>
@@ -2916,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1089</v>
       </c>
@@ -2948,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1090</v>
       </c>
@@ -2980,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1091</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1092</v>
       </c>
@@ -3044,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1093</v>
       </c>
@@ -3076,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1094</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1095</v>
       </c>
@@ -3140,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1096</v>
       </c>
@@ -3172,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1097</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1098</v>
       </c>
@@ -3242,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1099</v>
       </c>
@@ -3274,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1100</v>
       </c>
@@ -3306,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1101</v>
       </c>
@@ -3338,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1102</v>
       </c>
@@ -3370,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1103</v>
       </c>
@@ -3402,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1104</v>
       </c>
@@ -3437,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1105</v>
       </c>
@@ -3472,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1106</v>
       </c>
@@ -3504,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1107</v>
       </c>
@@ -3539,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1108</v>
       </c>
@@ -3574,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1109</v>
       </c>
@@ -3609,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1110</v>
       </c>
@@ -3644,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1111</v>
       </c>
@@ -3679,7 +3683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1112</v>
       </c>
@@ -3711,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1113</v>
       </c>
@@ -3743,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1114</v>
       </c>
@@ -3775,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1115</v>
       </c>
@@ -3810,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1116</v>
       </c>
@@ -3845,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1117</v>
       </c>
@@ -3877,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1118</v>
       </c>
@@ -3909,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1119</v>
       </c>
@@ -3941,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1120</v>
       </c>
@@ -3973,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1121</v>
       </c>
@@ -4008,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1122</v>
       </c>
@@ -4040,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1123</v>
       </c>
@@ -4072,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1124</v>
       </c>
@@ -4107,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1125</v>
       </c>
@@ -4139,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1126</v>
       </c>
@@ -4171,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>27</v>
       </c>
@@ -4203,11 +4207,11 @@
         <v>0</v>
       </c>
       <c r="P61" s="2" t="str">
-        <f>IF(C61=K61,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P61:P69" si="0">IF(C61=K61,"Y","N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6273</v>
       </c>
@@ -4239,11 +4243,11 @@
         <v>0</v>
       </c>
       <c r="P62" s="2" t="str">
-        <f>IF(C62=K62,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>28</v>
       </c>
@@ -4275,11 +4279,11 @@
         <v>0</v>
       </c>
       <c r="P63" s="2" t="str">
-        <f>IF(C63=K63,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>29</v>
       </c>
@@ -4311,11 +4315,11 @@
         <v>0</v>
       </c>
       <c r="P64" s="2" t="str">
-        <f>IF(C64=K64,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6272</v>
       </c>
@@ -4347,11 +4351,11 @@
         <v>0</v>
       </c>
       <c r="P65" s="2" t="str">
-        <f>IF(C65=K65,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>30</v>
       </c>
@@ -4383,11 +4387,11 @@
         <v>0</v>
       </c>
       <c r="P66" s="2" t="str">
-        <f>IF(C66=K66,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>31</v>
       </c>
@@ -4419,11 +4423,11 @@
         <v>0</v>
       </c>
       <c r="P67" s="2" t="str">
-        <f>IF(C67=K67,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>32</v>
       </c>
@@ -4455,11 +4459,11 @@
         <v>0</v>
       </c>
       <c r="P68" s="2" t="str">
-        <f>IF(C68=K68,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6271</v>
       </c>
@@ -4491,11 +4495,11 @@
         <v>0</v>
       </c>
       <c r="P69" s="2" t="str">
-        <f>IF(C69=K69,"Y","N")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1127</v>
       </c>
@@ -4521,11 +4525,11 @@
         <v>1</v>
       </c>
       <c r="P70" s="2" t="str">
-        <f>IF(C70=K70,"Y","")</f>
+        <f t="shared" ref="P70:P101" si="1">IF(C70=K70,"Y","")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1128</v>
       </c>
@@ -4551,11 +4555,11 @@
         <v>1</v>
       </c>
       <c r="P71" s="2" t="str">
-        <f>IF(C71=K71,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2524</v>
       </c>
@@ -4584,11 +4588,11 @@
         <v>0</v>
       </c>
       <c r="P72" s="2" t="str">
-        <f>IF(C72=K72,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1129</v>
       </c>
@@ -4614,11 +4618,11 @@
         <v>1</v>
       </c>
       <c r="P73" s="2" t="str">
-        <f>IF(C73=K73,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1130</v>
       </c>
@@ -4644,11 +4648,11 @@
         <v>1</v>
       </c>
       <c r="P74" s="2" t="str">
-        <f>IF(C74=K74,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1131</v>
       </c>
@@ -4680,11 +4684,11 @@
         <v>0</v>
       </c>
       <c r="P75" s="2" t="str">
-        <f>IF(C75=K75,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1132</v>
       </c>
@@ -4710,11 +4714,11 @@
         <v>1</v>
       </c>
       <c r="P76" s="2" t="str">
-        <f>IF(C76=K76,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1133</v>
       </c>
@@ -4746,11 +4750,11 @@
         <v>0</v>
       </c>
       <c r="P77" s="2" t="str">
-        <f>IF(C77=K77,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>5316</v>
       </c>
@@ -4776,11 +4780,11 @@
         <v>1</v>
       </c>
       <c r="P78" s="2" t="str">
-        <f>IF(C78=K78,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1134</v>
       </c>
@@ -4806,11 +4810,11 @@
         <v>1</v>
       </c>
       <c r="P79" s="2" t="str">
-        <f>IF(C79=K79,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1135</v>
       </c>
@@ -4836,11 +4840,11 @@
         <v>1</v>
       </c>
       <c r="P80" s="2" t="str">
-        <f>IF(C80=K80,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2525</v>
       </c>
@@ -4866,11 +4870,11 @@
         <v>1</v>
       </c>
       <c r="P81" s="2" t="str">
-        <f>IF(C81=K81,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1136</v>
       </c>
@@ -4896,11 +4900,11 @@
         <v>1</v>
       </c>
       <c r="P82" s="2" t="str">
-        <f>IF(C82=K82,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>5001</v>
       </c>
@@ -4932,11 +4936,11 @@
         <v>0</v>
       </c>
       <c r="P83" s="2" t="str">
-        <f>IF(C83=K83,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2169</v>
       </c>
@@ -4968,11 +4972,11 @@
         <v>0</v>
       </c>
       <c r="P84" s="2" t="str">
-        <f>IF(C84=K84,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2176</v>
       </c>
@@ -5004,11 +5008,11 @@
         <v>0</v>
       </c>
       <c r="P85" s="2" t="str">
-        <f>IF(C85=K85,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2177</v>
       </c>
@@ -5040,11 +5044,11 @@
         <v>0</v>
       </c>
       <c r="P86" s="2" t="str">
-        <f>IF(C86=K86,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2178</v>
       </c>
@@ -5076,11 +5080,11 @@
         <v>0</v>
       </c>
       <c r="P87" s="2" t="str">
-        <f>IF(C87=K87,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2179</v>
       </c>
@@ -5112,11 +5116,11 @@
         <v>0</v>
       </c>
       <c r="P88" s="2" t="str">
-        <f>IF(C88=K88,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2180</v>
       </c>
@@ -5148,11 +5152,11 @@
         <v>0</v>
       </c>
       <c r="P89" s="2" t="str">
-        <f>IF(C89=K89,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2181</v>
       </c>
@@ -5184,11 +5188,11 @@
         <v>0</v>
       </c>
       <c r="P90" s="2" t="str">
-        <f>IF(C90=K90,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>118</v>
       </c>
@@ -5223,11 +5227,11 @@
         <v>0</v>
       </c>
       <c r="P91" s="2" t="str">
-        <f>IF(C91=K91,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>119</v>
       </c>
@@ -5256,11 +5260,11 @@
         <v>1</v>
       </c>
       <c r="P92" s="2" t="str">
-        <f>IF(C92=K92,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>120</v>
       </c>
@@ -5289,11 +5293,11 @@
         <v>1</v>
       </c>
       <c r="P93" s="2" t="str">
-        <f>IF(C93=K93,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>121</v>
       </c>
@@ -5322,11 +5326,11 @@
         <v>1</v>
       </c>
       <c r="P94" s="2" t="str">
-        <f>IF(C94=K94,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>122</v>
       </c>
@@ -5355,11 +5359,11 @@
         <v>1</v>
       </c>
       <c r="P95" s="2" t="str">
-        <f>IF(C95=K95,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>123</v>
       </c>
@@ -5388,11 +5392,11 @@
         <v>1</v>
       </c>
       <c r="P96" s="2" t="str">
-        <f>IF(C96=K96,"Y","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1068</v>
       </c>
@@ -5427,11 +5431,11 @@
         <v>0</v>
       </c>
       <c r="P97" s="2" t="str">
-        <f>IF(C97=K97,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1069</v>
       </c>
@@ -5463,11 +5467,11 @@
         <v>0</v>
       </c>
       <c r="P98" s="2" t="str">
-        <f>IF(C98=K98,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1070</v>
       </c>
@@ -5499,11 +5503,11 @@
         <v>0</v>
       </c>
       <c r="P99" s="2" t="str">
-        <f>IF(C99=K99,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1071</v>
       </c>
@@ -5535,11 +5539,11 @@
         <v>0</v>
       </c>
       <c r="P100" s="2" t="str">
-        <f>IF(C100=K100,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1072</v>
       </c>
@@ -5571,11 +5575,11 @@
         <v>0</v>
       </c>
       <c r="P101" s="2" t="str">
-        <f>IF(C101=K101,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1073</v>
       </c>
@@ -5607,11 +5611,11 @@
         <v>0</v>
       </c>
       <c r="P102" s="2" t="str">
-        <f>IF(C102=K102,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P102:P133" si="2">IF(C102=K102,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1074</v>
       </c>
@@ -5646,11 +5650,11 @@
         <v>0</v>
       </c>
       <c r="P103" s="2" t="str">
-        <f>IF(C103=K103,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1075</v>
       </c>
@@ -5682,11 +5686,11 @@
         <v>0</v>
       </c>
       <c r="P104" s="2" t="str">
-        <f>IF(C104=K104,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1076</v>
       </c>
@@ -5718,11 +5722,11 @@
         <v>0</v>
       </c>
       <c r="P105" s="2" t="str">
-        <f>IF(C105=K105,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1077</v>
       </c>
@@ -5757,11 +5761,11 @@
         <v>0</v>
       </c>
       <c r="P106" s="2" t="str">
-        <f>IF(C106=K106,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1078</v>
       </c>
@@ -5793,11 +5797,11 @@
         <v>0</v>
       </c>
       <c r="P107" s="2" t="str">
-        <f>IF(C107=K107,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1079</v>
       </c>
@@ -5829,11 +5833,11 @@
         <v>0</v>
       </c>
       <c r="P108" s="2" t="str">
-        <f>IF(C108=K108,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1080</v>
       </c>
@@ -5865,11 +5869,11 @@
         <v>0</v>
       </c>
       <c r="P109" s="2" t="str">
-        <f>IF(C109=K109,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1081</v>
       </c>
@@ -5901,11 +5905,11 @@
         <v>0</v>
       </c>
       <c r="P110" s="2" t="str">
-        <f>IF(C110=K110,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1082</v>
       </c>
@@ -5937,11 +5941,11 @@
         <v>0</v>
       </c>
       <c r="P111" s="2" t="str">
-        <f>IF(C111=K111,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1083</v>
       </c>
@@ -5973,11 +5977,11 @@
         <v>0</v>
       </c>
       <c r="P112" s="2" t="str">
-        <f>IF(C112=K112,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1084</v>
       </c>
@@ -6009,11 +6013,11 @@
         <v>0</v>
       </c>
       <c r="P113" s="2" t="str">
-        <f>IF(C113=K113,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1085</v>
       </c>
@@ -6045,11 +6049,11 @@
         <v>0</v>
       </c>
       <c r="P114" s="2" t="str">
-        <f>IF(C114=K114,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1086</v>
       </c>
@@ -6081,11 +6085,11 @@
         <v>0</v>
       </c>
       <c r="P115" s="2" t="str">
-        <f>IF(C115=K115,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1087</v>
       </c>
@@ -6117,11 +6121,11 @@
         <v>0</v>
       </c>
       <c r="P116" s="2" t="str">
-        <f>IF(C116=K116,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1088</v>
       </c>
@@ -6153,11 +6157,11 @@
         <v>0</v>
       </c>
       <c r="P117" s="2" t="str">
-        <f>IF(C117=K117,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1089</v>
       </c>
@@ -6189,11 +6193,11 @@
         <v>0</v>
       </c>
       <c r="P118" s="2" t="str">
-        <f>IF(C118=K118,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1090</v>
       </c>
@@ -6225,11 +6229,11 @@
         <v>0</v>
       </c>
       <c r="P119" s="2" t="str">
-        <f>IF(C119=K119,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1091</v>
       </c>
@@ -6261,11 +6265,11 @@
         <v>0</v>
       </c>
       <c r="P120" s="2" t="str">
-        <f>IF(C120=K120,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1092</v>
       </c>
@@ -6297,11 +6301,11 @@
         <v>0</v>
       </c>
       <c r="P121" s="2" t="str">
-        <f>IF(C121=K121,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1093</v>
       </c>
@@ -6333,11 +6337,11 @@
         <v>0</v>
       </c>
       <c r="P122" s="2" t="str">
-        <f>IF(C122=K122,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1094</v>
       </c>
@@ -6369,11 +6373,11 @@
         <v>0</v>
       </c>
       <c r="P123" s="2" t="str">
-        <f>IF(C123=K123,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1095</v>
       </c>
@@ -6405,11 +6409,11 @@
         <v>0</v>
       </c>
       <c r="P124" s="2" t="str">
-        <f>IF(C124=K124,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1096</v>
       </c>
@@ -6441,11 +6445,11 @@
         <v>0</v>
       </c>
       <c r="P125" s="2" t="str">
-        <f>IF(C125=K125,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1097</v>
       </c>
@@ -6480,11 +6484,11 @@
         <v>0</v>
       </c>
       <c r="P126" s="2" t="str">
-        <f>IF(C126=K126,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1098</v>
       </c>
@@ -6519,11 +6523,11 @@
         <v>0</v>
       </c>
       <c r="P127" s="2" t="str">
-        <f>IF(C127=K127,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1099</v>
       </c>
@@ -6555,11 +6559,11 @@
         <v>0</v>
       </c>
       <c r="P128" s="2" t="str">
-        <f>IF(C128=K128,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1100</v>
       </c>
@@ -6591,11 +6595,11 @@
         <v>0</v>
       </c>
       <c r="P129" s="2" t="str">
-        <f>IF(C129=K129,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1101</v>
       </c>
@@ -6627,11 +6631,11 @@
         <v>0</v>
       </c>
       <c r="P130" s="2" t="str">
-        <f>IF(C130=K130,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1102</v>
       </c>
@@ -6663,11 +6667,11 @@
         <v>0</v>
       </c>
       <c r="P131" s="2" t="str">
-        <f>IF(C131=K131,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1103</v>
       </c>
@@ -6699,11 +6703,11 @@
         <v>0</v>
       </c>
       <c r="P132" s="2" t="str">
-        <f>IF(C132=K132,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1104</v>
       </c>
@@ -6738,11 +6742,11 @@
         <v>0</v>
       </c>
       <c r="P133" s="2" t="str">
-        <f>IF(C133=K133,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1105</v>
       </c>
@@ -6777,11 +6781,11 @@
         <v>0</v>
       </c>
       <c r="P134" s="2" t="str">
-        <f>IF(C134=K134,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P134:P165" si="3">IF(C134=K134,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1106</v>
       </c>
@@ -6813,11 +6817,11 @@
         <v>0</v>
       </c>
       <c r="P135" s="2" t="str">
-        <f>IF(C135=K135,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1107</v>
       </c>
@@ -6852,11 +6856,11 @@
         <v>0</v>
       </c>
       <c r="P136" s="2" t="str">
-        <f>IF(C136=K136,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1108</v>
       </c>
@@ -6891,11 +6895,11 @@
         <v>0</v>
       </c>
       <c r="P137" s="2" t="str">
-        <f>IF(C137=K137,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>1109</v>
       </c>
@@ -6930,11 +6934,11 @@
         <v>0</v>
       </c>
       <c r="P138" s="2" t="str">
-        <f>IF(C138=K138,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>1110</v>
       </c>
@@ -6969,11 +6973,11 @@
         <v>0</v>
       </c>
       <c r="P139" s="2" t="str">
-        <f>IF(C139=K139,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>1111</v>
       </c>
@@ -7008,11 +7012,11 @@
         <v>0</v>
       </c>
       <c r="P140" s="2" t="str">
-        <f>IF(C140=K140,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1112</v>
       </c>
@@ -7044,11 +7048,11 @@
         <v>0</v>
       </c>
       <c r="P141" s="2" t="str">
-        <f>IF(C141=K141,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1113</v>
       </c>
@@ -7080,11 +7084,11 @@
         <v>0</v>
       </c>
       <c r="P142" s="2" t="str">
-        <f>IF(C142=K142,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1114</v>
       </c>
@@ -7116,11 +7120,11 @@
         <v>0</v>
       </c>
       <c r="P143" s="2" t="str">
-        <f>IF(C143=K143,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1115</v>
       </c>
@@ -7155,11 +7159,11 @@
         <v>0</v>
       </c>
       <c r="P144" s="2" t="str">
-        <f>IF(C144=K144,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1116</v>
       </c>
@@ -7194,11 +7198,11 @@
         <v>0</v>
       </c>
       <c r="P145" s="2" t="str">
-        <f>IF(C145=K145,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1117</v>
       </c>
@@ -7230,11 +7234,11 @@
         <v>0</v>
       </c>
       <c r="P146" s="2" t="str">
-        <f>IF(C146=K146,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1118</v>
       </c>
@@ -7266,11 +7270,11 @@
         <v>0</v>
       </c>
       <c r="P147" s="2" t="str">
-        <f>IF(C147=K147,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1119</v>
       </c>
@@ -7302,11 +7306,11 @@
         <v>0</v>
       </c>
       <c r="P148" s="2" t="str">
-        <f>IF(C148=K148,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>1120</v>
       </c>
@@ -7338,11 +7342,11 @@
         <v>0</v>
       </c>
       <c r="P149" s="2" t="str">
-        <f>IF(C149=K149,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1121</v>
       </c>
@@ -7377,11 +7381,11 @@
         <v>0</v>
       </c>
       <c r="P150" s="2" t="str">
-        <f>IF(C150=K150,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1122</v>
       </c>
@@ -7413,11 +7417,11 @@
         <v>0</v>
       </c>
       <c r="P151" s="2" t="str">
-        <f>IF(C151=K151,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>1123</v>
       </c>
@@ -7449,11 +7453,11 @@
         <v>0</v>
       </c>
       <c r="P152" s="2" t="str">
-        <f>IF(C152=K152,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1124</v>
       </c>
@@ -7488,11 +7492,11 @@
         <v>0</v>
       </c>
       <c r="P153" s="2" t="str">
-        <f>IF(C153=K153,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>1125</v>
       </c>
@@ -7524,11 +7528,11 @@
         <v>0</v>
       </c>
       <c r="P154" s="2" t="str">
-        <f>IF(C154=K154,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>1126</v>
       </c>
@@ -7560,11 +7564,11 @@
         <v>0</v>
       </c>
       <c r="P155" s="2" t="str">
-        <f>IF(C155=K155,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2094</v>
       </c>
@@ -7596,11 +7600,11 @@
         <v>0</v>
       </c>
       <c r="P156" s="2" t="str">
-        <f>IF(C156=K156,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2095</v>
       </c>
@@ -7632,11 +7636,11 @@
         <v>0</v>
       </c>
       <c r="P157" s="2" t="str">
-        <f>IF(C157=K157,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>2096</v>
       </c>
@@ -7668,11 +7672,11 @@
         <v>0</v>
       </c>
       <c r="P158" s="2" t="str">
-        <f>IF(C158=K158,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>2097</v>
       </c>
@@ -7704,11 +7708,11 @@
         <v>0</v>
       </c>
       <c r="P159" s="2" t="str">
-        <f>IF(C159=K159,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>820</v>
       </c>
@@ -7746,11 +7750,11 @@
         <v>0</v>
       </c>
       <c r="P160" s="2" t="str">
-        <f>IF(C160=K160,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>821</v>
       </c>
@@ -7788,11 +7792,11 @@
         <v>0</v>
       </c>
       <c r="P161" s="2" t="str">
-        <f>IF(C161=K161,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>835</v>
       </c>
@@ -7830,11 +7834,11 @@
         <v>0</v>
       </c>
       <c r="P162" s="2" t="str">
-        <f>IF(C162=K162,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>5922</v>
       </c>
@@ -7872,11 +7876,11 @@
         <v>0</v>
       </c>
       <c r="P163" s="2" t="str">
-        <f>IF(C163=K163,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>827</v>
       </c>
@@ -7914,11 +7918,11 @@
         <v>0</v>
       </c>
       <c r="P164" s="2" t="str">
-        <f>IF(C164=K164,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>825</v>
       </c>
@@ -7956,11 +7960,11 @@
         <v>0</v>
       </c>
       <c r="P165" s="2" t="str">
-        <f>IF(C165=K165,"Y","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>824</v>
       </c>
@@ -7998,11 +8002,11 @@
         <v>0</v>
       </c>
       <c r="P166" s="2" t="str">
-        <f>IF(C166=K166,"Y","")</f>
+        <f t="shared" ref="P166:P197" si="4">IF(C166=K166,"Y","")</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>831</v>
       </c>
@@ -8040,11 +8044,11 @@
         <v>0</v>
       </c>
       <c r="P167" s="2" t="str">
-        <f>IF(C167=K167,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>832</v>
       </c>
@@ -8082,11 +8086,11 @@
         <v>0</v>
       </c>
       <c r="P168" s="2" t="str">
-        <f>IF(C168=K168,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>822</v>
       </c>
@@ -8124,11 +8128,11 @@
         <v>0</v>
       </c>
       <c r="P169" s="2" t="str">
-        <f>IF(C169=K169,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>833</v>
       </c>
@@ -8166,11 +8170,11 @@
         <v>0</v>
       </c>
       <c r="P170" s="2" t="str">
-        <f>IF(C170=K170,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>838</v>
       </c>
@@ -8208,11 +8212,11 @@
         <v>0</v>
       </c>
       <c r="P171" s="2" t="str">
-        <f>IF(C171=K171,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>823</v>
       </c>
@@ -8250,11 +8254,11 @@
         <v>0</v>
       </c>
       <c r="P172" s="2" t="str">
-        <f>IF(C172=K172,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>826</v>
       </c>
@@ -8292,11 +8296,11 @@
         <v>0</v>
       </c>
       <c r="P173" s="2" t="str">
-        <f>IF(C173=K173,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>6352</v>
       </c>
@@ -8334,11 +8338,11 @@
         <v>0</v>
       </c>
       <c r="P174" s="2" t="str">
-        <f>IF(C174=K174,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>836</v>
       </c>
@@ -8376,11 +8380,11 @@
         <v>0</v>
       </c>
       <c r="P175" s="2" t="str">
-        <f>IF(C175=K175,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>5923</v>
       </c>
@@ -8412,11 +8416,11 @@
         <v>0</v>
       </c>
       <c r="P176" s="2" t="str">
-        <f>IF(C176=K176,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>837</v>
       </c>
@@ -8454,11 +8458,11 @@
         <v>0</v>
       </c>
       <c r="P177" s="2" t="str">
-        <f>IF(C177=K177,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>829</v>
       </c>
@@ -8496,11 +8500,11 @@
         <v>0</v>
       </c>
       <c r="P178" s="2" t="str">
-        <f>IF(C178=K178,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>828</v>
       </c>
@@ -8532,11 +8536,11 @@
         <v>0</v>
       </c>
       <c r="P179" s="2" t="str">
-        <f>IF(C179=K179,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>6351</v>
       </c>
@@ -8568,11 +8572,11 @@
         <v>0</v>
       </c>
       <c r="P180" s="2" t="str">
-        <f>IF(C180=K180,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>839</v>
       </c>
@@ -8610,11 +8614,11 @@
         <v>0</v>
       </c>
       <c r="P181" s="2" t="str">
-        <f>IF(C181=K181,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>840</v>
       </c>
@@ -8652,11 +8656,11 @@
         <v>0</v>
       </c>
       <c r="P182" s="2" t="str">
-        <f>IF(C182=K182,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>841</v>
       </c>
@@ -8688,11 +8692,11 @@
         <v>0</v>
       </c>
       <c r="P183" s="2" t="str">
-        <f>IF(C183=K183,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>842</v>
       </c>
@@ -8730,11 +8734,11 @@
         <v>0</v>
       </c>
       <c r="P184" s="2" t="str">
-        <f>IF(C184=K184,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>843</v>
       </c>
@@ -8772,11 +8776,11 @@
         <v>0</v>
       </c>
       <c r="P185" s="2" t="str">
-        <f>IF(C185=K185,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>844</v>
       </c>
@@ -8814,11 +8818,11 @@
         <v>0</v>
       </c>
       <c r="P186" s="2" t="str">
-        <f>IF(C186=K186,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>3163</v>
       </c>
@@ -8853,11 +8857,11 @@
         <v>0</v>
       </c>
       <c r="P187" s="2" t="str">
-        <f>IF(C187=K187,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>830</v>
       </c>
@@ -8892,11 +8896,11 @@
         <v>0</v>
       </c>
       <c r="P188" s="2" t="str">
-        <f>IF(C188=K188,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>3162</v>
       </c>
@@ -8925,11 +8929,11 @@
         <v>0</v>
       </c>
       <c r="P189" s="2" t="str">
-        <f>IF(C189=K189,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>3164</v>
       </c>
@@ -8964,11 +8968,11 @@
         <v>0</v>
       </c>
       <c r="P190" s="2" t="str">
-        <f>IF(C190=K190,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>3165</v>
       </c>
@@ -9003,7 +9007,7 @@
         <v>0</v>
       </c>
       <c r="P191" s="2" t="str">
-        <f>IF(C191=K191,"Y","")</f>
+        <f t="shared" si="4"/>
         <v>Y</v>
       </c>
     </row>
@@ -9036,11 +9040,11 @@
         <v>0</v>
       </c>
       <c r="P192" s="2" t="str">
-        <f>IF(C192=K192,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>6453</v>
       </c>
@@ -9072,11 +9076,11 @@
         <v>0</v>
       </c>
       <c r="P193" s="2" t="str">
-        <f>IF(C193=K193,"Y","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>1248</v>
       </c>
@@ -9108,11 +9112,11 @@
         <v>0</v>
       </c>
       <c r="P194" s="2" t="str">
-        <f>IF(C194=K194,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>1249</v>
       </c>
@@ -9144,11 +9148,11 @@
         <v>0</v>
       </c>
       <c r="P195" s="2" t="str">
-        <f>IF(C195=K195,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>1250</v>
       </c>
@@ -9180,11 +9184,11 @@
         <v>0</v>
       </c>
       <c r="P196" s="2" t="str">
-        <f>IF(C196=K196,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>1251</v>
       </c>
@@ -9216,11 +9220,11 @@
         <v>0</v>
       </c>
       <c r="P197" s="2" t="str">
-        <f>IF(C197=K197,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>1252</v>
       </c>
@@ -9252,11 +9256,11 @@
         <v>0</v>
       </c>
       <c r="P198" s="2" t="str">
-        <f>IF(C198=K198,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P198:P227" si="5">IF(C198=K198,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>1253</v>
       </c>
@@ -9288,11 +9292,11 @@
         <v>0</v>
       </c>
       <c r="P199" s="2" t="str">
-        <f>IF(C199=K199,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>1254</v>
       </c>
@@ -9324,7 +9328,7 @@
         <v>0</v>
       </c>
       <c r="P200" s="2" t="str">
-        <f>IF(C200=K200,"Y","")</f>
+        <f t="shared" si="5"/>
         <v>Y</v>
       </c>
     </row>
@@ -9360,11 +9364,11 @@
         <v>1</v>
       </c>
       <c r="P201" s="2" t="str">
-        <f>IF(C201=K201,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1255</v>
       </c>
@@ -9396,11 +9400,11 @@
         <v>0</v>
       </c>
       <c r="P202" s="2" t="str">
-        <f>IF(C202=K202,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1267</v>
       </c>
@@ -9432,11 +9436,11 @@
         <v>0</v>
       </c>
       <c r="P203" s="2" t="str">
-        <f>IF(C203=K203,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1268</v>
       </c>
@@ -9468,11 +9472,11 @@
         <v>0</v>
       </c>
       <c r="P204" s="2" t="str">
-        <f>IF(C204=K204,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1256</v>
       </c>
@@ -9504,11 +9508,11 @@
         <v>0</v>
       </c>
       <c r="P205" s="2" t="str">
-        <f>IF(C205=K205,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1257</v>
       </c>
@@ -9540,11 +9544,11 @@
         <v>0</v>
       </c>
       <c r="P206" s="2" t="str">
-        <f>IF(C206=K206,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1258</v>
       </c>
@@ -9576,11 +9580,11 @@
         <v>0</v>
       </c>
       <c r="P207" s="2" t="str">
-        <f>IF(C207=K207,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>3199</v>
       </c>
@@ -9612,11 +9616,11 @@
         <v>0</v>
       </c>
       <c r="P208" s="2" t="str">
-        <f>IF(C208=K208,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1259</v>
       </c>
@@ -9648,11 +9652,11 @@
         <v>0</v>
       </c>
       <c r="P209" s="2" t="str">
-        <f>IF(C209=K209,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>1260</v>
       </c>
@@ -9684,11 +9688,11 @@
         <v>0</v>
       </c>
       <c r="P210" s="2" t="str">
-        <f>IF(C210=K210,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>1261</v>
       </c>
@@ -9720,11 +9724,11 @@
         <v>0</v>
       </c>
       <c r="P211" s="2" t="str">
-        <f>IF(C211=K211,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>1262</v>
       </c>
@@ -9756,11 +9760,11 @@
         <v>0</v>
       </c>
       <c r="P212" s="2" t="str">
-        <f>IF(C212=K212,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>1263</v>
       </c>
@@ -9792,11 +9796,11 @@
         <v>0</v>
       </c>
       <c r="P213" s="2" t="str">
-        <f>IF(C213=K213,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>1264</v>
       </c>
@@ -9828,11 +9832,11 @@
         <v>0</v>
       </c>
       <c r="P214" s="2" t="str">
-        <f>IF(C214=K214,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1265</v>
       </c>
@@ -9864,11 +9868,11 @@
         <v>0</v>
       </c>
       <c r="P215" s="2" t="str">
-        <f>IF(C215=K215,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1266</v>
       </c>
@@ -9900,11 +9904,11 @@
         <v>0</v>
       </c>
       <c r="P216" s="2" t="str">
-        <f>IF(C216=K216,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>1269</v>
       </c>
@@ -9936,11 +9940,11 @@
         <v>0</v>
       </c>
       <c r="P217" s="2" t="str">
-        <f>IF(C217=K217,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>1270</v>
       </c>
@@ -9972,11 +9976,11 @@
         <v>0</v>
       </c>
       <c r="P218" s="2" t="str">
-        <f>IF(C218=K218,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>3200</v>
       </c>
@@ -10008,11 +10012,11 @@
         <v>0</v>
       </c>
       <c r="P219" s="2" t="str">
-        <f>IF(C219=K219,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>1271</v>
       </c>
@@ -10044,11 +10048,11 @@
         <v>0</v>
       </c>
       <c r="P220" s="2" t="str">
-        <f>IF(C220=K220,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>1272</v>
       </c>
@@ -10080,11 +10084,11 @@
         <v>0</v>
       </c>
       <c r="P221" s="2" t="str">
-        <f>IF(C221=K221,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>1273</v>
       </c>
@@ -10116,11 +10120,11 @@
         <v>0</v>
       </c>
       <c r="P222" s="2" t="str">
-        <f>IF(C222=K222,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>1274</v>
       </c>
@@ -10152,11 +10156,11 @@
         <v>0</v>
       </c>
       <c r="P223" s="2" t="str">
-        <f>IF(C223=K223,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>1275</v>
       </c>
@@ -10188,11 +10192,11 @@
         <v>0</v>
       </c>
       <c r="P224" s="2" t="str">
-        <f>IF(C224=K224,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>1276</v>
       </c>
@@ -10224,11 +10228,11 @@
         <v>0</v>
       </c>
       <c r="P225" s="2" t="str">
-        <f>IF(C225=K225,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>1277</v>
       </c>
@@ -10260,11 +10264,11 @@
         <v>0</v>
       </c>
       <c r="P226" s="2" t="str">
-        <f>IF(C226=K226,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>1278</v>
       </c>
@@ -10296,11 +10300,11 @@
         <v>0</v>
       </c>
       <c r="P227" s="2" t="str">
-        <f>IF(C227=K227,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>827</v>
       </c>
@@ -10344,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>825</v>
       </c>
@@ -10388,7 +10392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>824</v>
       </c>
@@ -10432,7 +10436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>831</v>
       </c>
@@ -10476,7 +10480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>832</v>
       </c>
@@ -10520,7 +10524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>822</v>
       </c>
@@ -10565,7 +10569,7 @@
       </c>
       <c r="R233" s="6"/>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>833</v>
       </c>
@@ -10609,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>838</v>
       </c>
@@ -10653,7 +10657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>3162</v>
       </c>
@@ -10694,7 +10698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>3164</v>
       </c>
@@ -10735,7 +10739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>3165</v>
       </c>
@@ -10776,7 +10780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>840</v>
       </c>
@@ -10820,7 +10824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>841</v>
       </c>
@@ -10864,7 +10868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>842</v>
       </c>
@@ -10908,7 +10912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>843</v>
       </c>
@@ -10952,7 +10956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>844</v>
       </c>
@@ -10996,7 +11000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>6401</v>
       </c>
@@ -11028,11 +11032,11 @@
         <v>0</v>
       </c>
       <c r="P244" s="2" t="str">
-        <f>IF(C244=K244,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P244:P275" si="6">IF(C244=K244,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>6402</v>
       </c>
@@ -11064,11 +11068,11 @@
         <v>0</v>
       </c>
       <c r="P245" s="2" t="str">
-        <f>IF(C245=K245,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>6403</v>
       </c>
@@ -11100,11 +11104,11 @@
         <v>0</v>
       </c>
       <c r="P246" s="2" t="str">
-        <f>IF(C246=K246,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>6404</v>
       </c>
@@ -11136,11 +11140,11 @@
         <v>0</v>
       </c>
       <c r="P247" s="2" t="str">
-        <f>IF(C247=K247,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>6405</v>
       </c>
@@ -11172,11 +11176,11 @@
         <v>0</v>
       </c>
       <c r="P248" s="2" t="str">
-        <f>IF(C248=K248,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>6406</v>
       </c>
@@ -11208,11 +11212,11 @@
         <v>0</v>
       </c>
       <c r="P249" s="2" t="str">
-        <f>IF(C249=K249,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>6407</v>
       </c>
@@ -11244,11 +11248,11 @@
         <v>0</v>
       </c>
       <c r="P250" s="2" t="str">
-        <f>IF(C250=K250,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>6408</v>
       </c>
@@ -11280,11 +11284,11 @@
         <v>0</v>
       </c>
       <c r="P251" s="2" t="str">
-        <f>IF(C251=K251,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>6409</v>
       </c>
@@ -11316,11 +11320,11 @@
         <v>0</v>
       </c>
       <c r="P252" s="2" t="str">
-        <f>IF(C252=K252,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>5378</v>
       </c>
@@ -11354,11 +11358,11 @@
         <v>0</v>
       </c>
       <c r="P253" s="2" t="str">
-        <f>IF(C253=K253,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>5375</v>
       </c>
@@ -11392,11 +11396,11 @@
         <v>0</v>
       </c>
       <c r="P254" s="2" t="str">
-        <f>IF(C254=K254,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>408</v>
       </c>
@@ -11430,11 +11434,11 @@
         <v>0</v>
       </c>
       <c r="P255" s="2" t="str">
-        <f>IF(C255=K255,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>409</v>
       </c>
@@ -11468,11 +11472,11 @@
         <v>0</v>
       </c>
       <c r="P256" s="2" t="str">
-        <f>IF(C256=K256,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>410</v>
       </c>
@@ -11506,11 +11510,11 @@
         <v>0</v>
       </c>
       <c r="P257" s="2" t="str">
-        <f>IF(C257=K257,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1516</v>
       </c>
@@ -11544,11 +11548,11 @@
         <v>0</v>
       </c>
       <c r="P258" s="2" t="str">
-        <f>IF(C258=K258,"Y","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1517</v>
       </c>
@@ -11582,11 +11586,11 @@
         <v>0</v>
       </c>
       <c r="P259" s="2" t="str">
-        <f>IF(C259=K259,"Y","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1518</v>
       </c>
@@ -11620,11 +11624,11 @@
         <v>0</v>
       </c>
       <c r="P260" s="2" t="str">
-        <f>IF(C260=K260,"Y","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1519</v>
       </c>
@@ -11658,11 +11662,11 @@
         <v>0</v>
       </c>
       <c r="P261" s="2" t="str">
-        <f>IF(C261=K261,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1520</v>
       </c>
@@ -11696,11 +11700,11 @@
         <v>0</v>
       </c>
       <c r="P262" s="2" t="str">
-        <f>IF(C262=K262,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1521</v>
       </c>
@@ -11726,11 +11730,11 @@
         <v>0</v>
       </c>
       <c r="P263" s="2" t="str">
-        <f>IF(C263=K263,"Y","")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1824</v>
       </c>
@@ -11767,11 +11771,11 @@
         <v>0</v>
       </c>
       <c r="P264" s="2" t="str">
-        <f>IF(C264=K264,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1823</v>
       </c>
@@ -11808,11 +11812,11 @@
         <v>0</v>
       </c>
       <c r="P265" s="2" t="str">
-        <f>IF(C265=K265,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1825</v>
       </c>
@@ -11849,11 +11853,11 @@
         <v>0</v>
       </c>
       <c r="P266" s="2" t="str">
-        <f>IF(C266=K266,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1827</v>
       </c>
@@ -11890,11 +11894,11 @@
         <v>0</v>
       </c>
       <c r="P267" s="2" t="str">
-        <f>IF(C267=K267,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1826</v>
       </c>
@@ -11931,11 +11935,11 @@
         <v>0</v>
       </c>
       <c r="P268" s="2" t="str">
-        <f>IF(C268=K268,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1828</v>
       </c>
@@ -11970,11 +11974,11 @@
         <v>0</v>
       </c>
       <c r="P269" s="2" t="str">
-        <f>IF(C269=K269,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1832</v>
       </c>
@@ -12009,11 +12013,11 @@
         <v>0</v>
       </c>
       <c r="P270" s="2" t="str">
-        <f>IF(C270=K270,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1830</v>
       </c>
@@ -12048,11 +12052,11 @@
         <v>0</v>
       </c>
       <c r="P271" s="2" t="str">
-        <f>IF(C271=K271,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="272" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1831</v>
       </c>
@@ -12087,11 +12091,11 @@
         <v>0</v>
       </c>
       <c r="P272" s="2" t="str">
-        <f>IF(C272=K272,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1834</v>
       </c>
@@ -12126,11 +12130,11 @@
         <v>0</v>
       </c>
       <c r="P273" s="2" t="str">
-        <f>IF(C273=K273,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1833</v>
       </c>
@@ -12165,11 +12169,11 @@
         <v>0</v>
       </c>
       <c r="P274" s="2" t="str">
-        <f>IF(C274=K274,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1835</v>
       </c>
@@ -12204,11 +12208,11 @@
         <v>0</v>
       </c>
       <c r="P275" s="2" t="str">
-        <f>IF(C275=K275,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1836</v>
       </c>
@@ -12243,11 +12247,11 @@
         <v>0</v>
       </c>
       <c r="P276" s="2" t="str">
-        <f>IF(C276=K276,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P276:P307" si="7">IF(C276=K276,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1837</v>
       </c>
@@ -12282,11 +12286,11 @@
         <v>0</v>
       </c>
       <c r="P277" s="2" t="str">
-        <f>IF(C277=K277,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1838</v>
       </c>
@@ -12321,11 +12325,11 @@
         <v>0</v>
       </c>
       <c r="P278" s="2" t="str">
-        <f>IF(C278=K278,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1840</v>
       </c>
@@ -12360,11 +12364,11 @@
         <v>0</v>
       </c>
       <c r="P279" s="2" t="str">
-        <f>IF(C279=K279,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1841</v>
       </c>
@@ -12399,11 +12403,11 @@
         <v>0</v>
       </c>
       <c r="P280" s="2" t="str">
-        <f>IF(C280=K280,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1842</v>
       </c>
@@ -12438,11 +12442,11 @@
         <v>0</v>
       </c>
       <c r="P281" s="2" t="str">
-        <f>IF(C281=K281,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1839</v>
       </c>
@@ -12477,11 +12481,11 @@
         <v>0</v>
       </c>
       <c r="P282" s="2" t="str">
-        <f>IF(C282=K282,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1843</v>
       </c>
@@ -12516,11 +12520,11 @@
         <v>0</v>
       </c>
       <c r="P283" s="2" t="str">
-        <f>IF(C283=K283,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1844</v>
       </c>
@@ -12555,11 +12559,11 @@
         <v>0</v>
       </c>
       <c r="P284" s="2" t="str">
-        <f>IF(C284=K284,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1845</v>
       </c>
@@ -12594,11 +12598,11 @@
         <v>0</v>
       </c>
       <c r="P285" s="2" t="str">
-        <f>IF(C285=K285,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1848</v>
       </c>
@@ -12633,11 +12637,11 @@
         <v>0</v>
       </c>
       <c r="P286" s="2" t="str">
-        <f>IF(C286=K286,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1847</v>
       </c>
@@ -12672,11 +12676,11 @@
         <v>0</v>
       </c>
       <c r="P287" s="2" t="str">
-        <f>IF(C287=K287,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1846</v>
       </c>
@@ -12711,11 +12715,11 @@
         <v>0</v>
       </c>
       <c r="P288" s="2" t="str">
-        <f>IF(C288=K288,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1849</v>
       </c>
@@ -12750,11 +12754,11 @@
         <v>0</v>
       </c>
       <c r="P289" s="2" t="str">
-        <f>IF(C289=K289,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1850</v>
       </c>
@@ -12789,11 +12793,11 @@
         <v>0</v>
       </c>
       <c r="P290" s="2" t="str">
-        <f>IF(C290=K290,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1852</v>
       </c>
@@ -12828,11 +12832,11 @@
         <v>0</v>
       </c>
       <c r="P291" s="2" t="str">
-        <f>IF(C291=K291,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="292" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1851</v>
       </c>
@@ -12867,11 +12871,11 @@
         <v>0</v>
       </c>
       <c r="P292" s="2" t="str">
-        <f>IF(C292=K292,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1853</v>
       </c>
@@ -12906,11 +12910,11 @@
         <v>0</v>
       </c>
       <c r="P293" s="2" t="str">
-        <f>IF(C293=K293,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1856</v>
       </c>
@@ -12945,11 +12949,11 @@
         <v>0</v>
       </c>
       <c r="P294" s="2" t="str">
-        <f>IF(C294=K294,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1860</v>
       </c>
@@ -12984,11 +12988,11 @@
         <v>0</v>
       </c>
       <c r="P295" s="2" t="str">
-        <f>IF(C295=K295,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="296" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1857</v>
       </c>
@@ -13023,11 +13027,11 @@
         <v>0</v>
       </c>
       <c r="P296" s="2" t="str">
-        <f>IF(C296=K296,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1858</v>
       </c>
@@ -13062,11 +13066,11 @@
         <v>0</v>
       </c>
       <c r="P297" s="2" t="str">
-        <f>IF(C297=K297,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="298" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1859</v>
       </c>
@@ -13101,11 +13105,11 @@
         <v>0</v>
       </c>
       <c r="P298" s="2" t="str">
-        <f>IF(C298=K298,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1861</v>
       </c>
@@ -13140,11 +13144,11 @@
         <v>0</v>
       </c>
       <c r="P299" s="2" t="str">
-        <f>IF(C299=K299,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1854</v>
       </c>
@@ -13179,11 +13183,11 @@
         <v>0</v>
       </c>
       <c r="P300" s="2" t="str">
-        <f>IF(C300=K300,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1855</v>
       </c>
@@ -13218,11 +13222,11 @@
         <v>0</v>
       </c>
       <c r="P301" s="2" t="str">
-        <f>IF(C301=K301,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>1829</v>
       </c>
@@ -13257,11 +13261,11 @@
         <v>0</v>
       </c>
       <c r="P302" s="2" t="str">
-        <f>IF(C302=K302,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>1862</v>
       </c>
@@ -13296,11 +13300,11 @@
         <v>0</v>
       </c>
       <c r="P303" s="2" t="str">
-        <f>IF(C303=K303,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>1863</v>
       </c>
@@ -13335,11 +13339,11 @@
         <v>0</v>
       </c>
       <c r="P304" s="2" t="str">
-        <f>IF(C304=K304,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>1864</v>
       </c>
@@ -13374,11 +13378,11 @@
         <v>0</v>
       </c>
       <c r="P305" s="2" t="str">
-        <f>IF(C305=K305,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>1865</v>
       </c>
@@ -13413,11 +13417,11 @@
         <v>0</v>
       </c>
       <c r="P306" s="2" t="str">
-        <f>IF(C306=K306,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>1866</v>
       </c>
@@ -13452,11 +13456,11 @@
         <v>0</v>
       </c>
       <c r="P307" s="2" t="str">
-        <f>IF(C307=K307,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>1867</v>
       </c>
@@ -13491,11 +13495,11 @@
         <v>0</v>
       </c>
       <c r="P308" s="2" t="str">
-        <f>IF(C308=K308,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" ref="P308:P321" si="8">IF(C308=K308,"Y","")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>1868</v>
       </c>
@@ -13530,11 +13534,11 @@
         <v>0</v>
       </c>
       <c r="P309" s="2" t="str">
-        <f>IF(C309=K309,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>1869</v>
       </c>
@@ -13569,11 +13573,11 @@
         <v>0</v>
       </c>
       <c r="P310" s="2" t="str">
-        <f>IF(C310=K310,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>1870</v>
       </c>
@@ -13608,11 +13612,11 @@
         <v>0</v>
       </c>
       <c r="P311" s="2" t="str">
-        <f>IF(C311=K311,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="312" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>1872</v>
       </c>
@@ -13647,11 +13651,11 @@
         <v>0</v>
       </c>
       <c r="P312" s="2" t="str">
-        <f>IF(C312=K312,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>1871</v>
       </c>
@@ -13686,11 +13690,11 @@
         <v>0</v>
       </c>
       <c r="P313" s="2" t="str">
-        <f>IF(C313=K313,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>1873</v>
       </c>
@@ -13725,11 +13729,11 @@
         <v>0</v>
       </c>
       <c r="P314" s="2" t="str">
-        <f>IF(C314=K314,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>1876</v>
       </c>
@@ -13764,11 +13768,11 @@
         <v>0</v>
       </c>
       <c r="P315" s="2" t="str">
-        <f>IF(C315=K315,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>1875</v>
       </c>
@@ -13803,11 +13807,11 @@
         <v>0</v>
       </c>
       <c r="P316" s="2" t="str">
-        <f>IF(C316=K316,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>1874</v>
       </c>
@@ -13842,11 +13846,11 @@
         <v>0</v>
       </c>
       <c r="P317" s="2" t="str">
-        <f>IF(C317=K317,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>1877</v>
       </c>
@@ -13881,11 +13885,11 @@
         <v>0</v>
       </c>
       <c r="P318" s="2" t="str">
-        <f>IF(C318=K318,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>1879</v>
       </c>
@@ -13920,11 +13924,11 @@
         <v>0</v>
       </c>
       <c r="P319" s="2" t="str">
-        <f>IF(C319=K319,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="320" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>1878</v>
       </c>
@@ -13959,11 +13963,11 @@
         <v>0</v>
       </c>
       <c r="P320" s="2" t="str">
-        <f>IF(C320=K320,"Y","")</f>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>1880</v>
       </c>
@@ -13998,12 +14002,17 @@
         <v>0</v>
       </c>
       <c r="P321" s="2" t="str">
-        <f>IF(C321=K321,"Y","")</f>
+        <f t="shared" si="8"/>
         <v>Y</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P321">
+  <autoFilter ref="A1:P321" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:O321">
       <sortCondition ref="I1:I321"/>
     </sortState>
@@ -14014,7 +14023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
@@ -14501,7 +14510,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B60">
+  <autoFilter ref="A1:B60" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:B59">
       <sortCondition ref="B1:B60"/>
     </sortState>

</xml_diff>